<commit_message>
[Update] 밸런스 조정 10:22
</commit_message>
<xml_diff>
--- a/Assets/Resource/Xlsx/GameData.xlsx
+++ b/Assets/Resource/Xlsx/GameData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Desktop\github\ProjectOz\Assets\Resource\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Desktop\Project_Oz\ProjectOz\Assets\Resource\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="20655" windowHeight="11295" tabRatio="760" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="20655" windowHeight="11295" tabRatio="760" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Pc" sheetId="1" r:id="rId1"/>
@@ -2668,7 +2668,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3635,8 +3635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3810,7 +3810,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>51</v>
@@ -5046,7 +5046,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5223,7 +5223,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5430,7 +5432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -5509,7 +5511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5664,7 +5668,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5751,7 +5755,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="H3" s="3">
         <v>30</v>

</xml_diff>